<commit_message>
Added support for extent report
Added support for extent report
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace\FrameworkDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LambdaCertification\FrameworkDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031A0BA-5571-45A6-A50A-7062D8545D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718572D3-0DEB-4029-A541-546CF7ACE1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4E2F37B-1189-4A76-A387-4B415CD000BB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A4E2F37B-1189-4A76-A387-4B415CD000BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Password</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>TestCase1_Login</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
   </si>
   <si>
     <t>female</t>
-  </si>
-  <si>
-    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -520,19 +514,19 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -543,42 +537,42 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
       <c r="N1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -587,18 +581,18 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -607,101 +601,101 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" t="s">
         <v>40</v>
       </c>
-      <c r="M5" t="s">
-        <v>41</v>
-      </c>
       <c r="N5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed changes of extent report with logs
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LambdaCertification\FrameworkDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718572D3-0DEB-4029-A541-546CF7ACE1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E04455-0331-4BBD-BD9E-45F5038CB07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{A4E2F37B-1189-4A76-A387-4B415CD000BB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Password</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F5"/>
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -607,7 +610,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
@@ -627,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -671,7 +674,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>17</v>

</xml_diff>